<commit_message>
Russian and other translations
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t xml:space="preserve">Message id</t>
   </si>
@@ -40,21 +40,30 @@
     <t xml:space="preserve">ARTE Taxi</t>
   </si>
   <si>
-    <t xml:space="preserve">Arte Taxisky</t>
+    <t xml:space="preserve">ARTE Taxi </t>
   </si>
   <si>
     <t xml:space="preserve">Autonoleggio RadioTaxi Terme Euganee</t>
   </si>
   <si>
+    <t xml:space="preserve">прокат автомобилей радио такси Terme Euganee </t>
+  </si>
+  <si>
     <t xml:space="preserve">Car rental RadioTaxi Terme Euganee</t>
   </si>
   <si>
     <t xml:space="preserve">A.R.T.E.</t>
   </si>
   <si>
+    <t xml:space="preserve">A.R.T.E</t>
+  </si>
+  <si>
     <t xml:space="preserve">Autonoleggio Radio Taxi</t>
   </si>
   <si>
+    <t xml:space="preserve">прокат автомобилей радио такси</t>
+  </si>
+  <si>
     <t xml:space="preserve">Car rental RadioTaxi</t>
   </si>
   <si>
@@ -64,6 +73,9 @@
     <t xml:space="preserve">Quem Somos</t>
   </si>
   <si>
+    <t xml:space="preserve">кто мы</t>
+  </si>
+  <si>
     <t xml:space="preserve">About us</t>
   </si>
   <si>
@@ -73,6 +85,9 @@
     <t xml:space="preserve">Serviços</t>
   </si>
   <si>
+    <t xml:space="preserve">обслуживание</t>
+  </si>
+  <si>
     <t xml:space="preserve">Services</t>
   </si>
   <si>
@@ -82,6 +97,9 @@
     <t xml:space="preserve">Carros</t>
   </si>
   <si>
+    <t xml:space="preserve">автомобиль</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cars</t>
   </si>
   <si>
@@ -91,10 +109,16 @@
     <t xml:space="preserve">Contatos</t>
   </si>
   <si>
+    <t xml:space="preserve">контакты</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contacts</t>
   </si>
   <si>
     <t xml:space="preserve">ARTE Taxi - Terme Euganee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTE Taxi Terme Euganee</t>
   </si>
   <si>
     <t xml:space="preserve">Il Consorzio Autonoleggio Radiotaxi Terme Euganee
@@ -110,7 +134,10 @@
 Oferecendo aos seus clientes carros luxuosos e elegantes, afim de oferecer máxima garantia de qualidade ,pontualidade,preço honesto e transparente com tarifas acessivéis, sempre previamente concordadas</t>
   </si>
   <si>
-    <t xml:space="preserve">The Radiotaxi Terme Terme Euganee Consortium carries out prestigious passenger cars in the TAXI and NCC (hire with driver) sector, always aiming to offer its customers the highest quality guarantee, punctuality, transparent price with rates agreed in advance</t>
+    <t xml:space="preserve">Консорциум Прокат автомобилей с водителем Радиотакси Терме Эуганее включает в себя операторов отрасли Taxi и CNN (прокат машины с водителем). Мы гарантируем своим клиентам великолепное качество обслуживания, пунктуальность, прозрачные цены по предварительно обговоренным тарифам, обслуживание на престижных моделях автомобилей.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Radiotaxi Terme Terme Euganee Consortium has a prestigious selection of passenger cars in the TAXI and hire with driver sector, always aiming to guarantee its customers the higest quality, punctuality and transparent prices with rates agreed in advance.</t>
   </si>
   <si>
     <t xml:space="preserve">Abbiamo ciò di cui hai bisogno</t>
@@ -119,7 +146,10 @@
     <t xml:space="preserve">TEMOS O QUE VOCÊ PRECISA</t>
   </si>
   <si>
-    <t xml:space="preserve">We have what you need</t>
+    <t xml:space="preserve">У нас вы найдете  все то, что ищете!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have everything you need</t>
   </si>
   <si>
     <t xml:space="preserve">I punti di forza del nostro gruppo sono una vasta gamma di automezzi,
@@ -135,11 +165,15 @@
 Sempre com um team de motoristas que estão há muitos anos no mercado de táxi ,com um amplo conhecimento do próprio território.</t>
   </si>
   <si>
+    <t xml:space="preserve">Сильные точки нашей группы являются самыми разнообразными транспортными средствами,  Berlina (седан) для деловых встреч, Station Wagon и минивэны для семейных поездок, микроавтобусы на 8 мест для групп, автомобили для перевозки инвалидов,  в любом месте назначения.  Еще одним важным преимуществом является то, что наши водители обладают многолетним опытом вождения и отличным знанием местности. 
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">The strengths of our group are a wide range of vehicles,
-the Berline for your business trips, our Station Wagon and Mopeds,
+Our sedans for your business trips, our Station Wagon and Minivans,
 our eight-seater minibuses and our disabled vehicle to go
-wherever you want, without leaving a team of drivers operating now
-for years in the sector with the utmost knowledge of the territory.</t>
+wherever you want, without forgetting a team of drivers who have been operating in the sector 
+for years  with an utmost knowledge of the territory.</t>
   </si>
   <si>
     <t xml:space="preserve">Assicuriamo la nostra puntuale presenza ovunque Voi lo richiediate
@@ -153,10 +187,14 @@
 Estaremos a disposição e será um prazer recebê-los para oferecer outras informações e realizar a sua exigência.</t>
   </si>
   <si>
+    <t xml:space="preserve">Мы гарантируем круглосуточное обслуживание в любое время года в любом месте Вашего нахождения.  По Вашему дополнительному запросу мы предоставим водителей со знанием английского, французского и немецкого языков. Будем рады предоставить Вам наши услуги и, в случае необходимости, любую дополнительную информацию
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">We assure our punctual presence wherever you request it
-24 hours a day for 365 days and on request we provide drivers with
+24 hours a day for 365 days a year and on request we provide drivers with
 knowledge of English, French and German.
-We will be delighted to offer you more information by putting all of it
+We would be delighted to offer you more information, putting all of it
 our experience at your disposal.</t>
   </si>
   <si>
@@ -166,7 +204,10 @@
     <t xml:space="preserve">para oferecer outras informações e realizar a sua exigência.</t>
   </si>
   <si>
-    <t xml:space="preserve">Everything to satisfy all your needs.</t>
+    <t xml:space="preserve">Все, чтобы удовлетворить все ваши потребности.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everything to satisfy  your needs.</t>
   </si>
   <si>
     <t xml:space="preserve">Vienici a trovare!</t>
@@ -175,7 +216,10 @@
     <t xml:space="preserve">Venha nos visitar,seremos felizes em conhece-lo!</t>
   </si>
   <si>
-    <t xml:space="preserve">Come to find us!</t>
+    <t xml:space="preserve">Мы ждем Вас!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come and se  us!</t>
   </si>
   <si>
     <t xml:space="preserve">Al tuo servizio</t>
@@ -184,6 +228,9 @@
     <t xml:space="preserve">AO TEU SERVIÇO</t>
   </si>
   <si>
+    <t xml:space="preserve">В Вашем распоряжении:</t>
+  </si>
+  <si>
     <t xml:space="preserve">At your service</t>
   </si>
   <si>
@@ -193,6 +240,9 @@
     <t xml:space="preserve">SERVIÇO TÁXI</t>
   </si>
   <si>
+    <t xml:space="preserve">Сервис такси</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taxi Service</t>
   </si>
   <si>
@@ -202,6 +252,9 @@
     <t xml:space="preserve">O melhor transporte de passageiros público</t>
   </si>
   <si>
+    <t xml:space="preserve">Для лучшего транспортного обслуживания</t>
+  </si>
+  <si>
     <t xml:space="preserve">The best public transport</t>
   </si>
   <si>
@@ -211,6 +264,9 @@
     <t xml:space="preserve">VIAGEM DE NEGÓCIOS</t>
   </si>
   <si>
+    <t xml:space="preserve">Деловые поездки</t>
+  </si>
+  <si>
     <t xml:space="preserve">Business travel</t>
   </si>
   <si>
@@ -220,6 +276,9 @@
     <t xml:space="preserve">Pensa ao teu business, na viagem pensamos nós</t>
   </si>
   <si>
+    <t xml:space="preserve">Сосредоточьтесь на своем бизнесе, об остальном позаботимся мы</t>
+  </si>
+  <si>
     <t xml:space="preserve">Focus on your business, we will think on the travel</t>
   </si>
   <si>
@@ -227,6 +286,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOURS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Туры</t>
   </si>
   <si>
     <t xml:space="preserve">Visite in città ed escursioni turistiche con possibilità di prenotazione
@@ -236,6 +298,9 @@
     <t xml:space="preserve">Visitas e excursões turísticas com possibilidade de fazer reserva de um guia turístico</t>
   </si>
   <si>
+    <t xml:space="preserve">Городские туры и туристические экскурсии с возможностью бронирования гида</t>
+  </si>
+  <si>
     <t xml:space="preserve">City tours and tourist excursions with possibility of booking a guide</t>
   </si>
   <si>
@@ -243,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">TRANSFERIMENTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Транспортный трансфер</t>
   </si>
   <si>
     <t xml:space="preserve">Transfers</t>
@@ -257,6 +325,9 @@
 Treviso e Venezia de modo fácil.De Táxi ou minibus.Oferecendo também serviços condivisos com outros passageiros</t>
   </si>
   <si>
+    <t xml:space="preserve">В аэропорты/ и на вокзалы/с Возможен групповой трансфер в близжайшие города Венецию и Тревизо</t>
+  </si>
+  <si>
     <t xml:space="preserve">From and to airports or stations&lt;br&gt;
 Treviso and Venice at your fingertips
 even with collective services</t>
@@ -265,16 +336,25 @@
     <t xml:space="preserve">VEDI</t>
   </si>
   <si>
+    <t xml:space="preserve">Просмотр</t>
+  </si>
+  <si>
     <t xml:space="preserve">VIEW</t>
   </si>
   <si>
     <t xml:space="preserve">Contattaci</t>
   </si>
   <si>
+    <t xml:space="preserve">Ждем ваших обращений!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contact us</t>
   </si>
   <si>
     <t xml:space="preserve">Consorzio Autonoleggio Radiotaxi Terme Euganee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">прокат автомобилей радио такси  Terme Euganee</t>
   </si>
   <si>
     <t xml:space="preserve">Car Rental Radiotaxi Terme Euganee</t>
@@ -292,10 +372,13 @@
 				Tel: 049.66.78.42</t>
   </si>
   <si>
+    <t xml:space="preserve">главный офис &lt;br&gt;     Via P. D'Abano 14&lt;br&gt;     35031 - Abano Terme - (PD)&lt;br&gt;     Tel: 049.66.78.42</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAIN OFFICE&lt;br&gt;
-				Via P. D'Abano 14&lt;br&gt;
-				35031 - Abano Terme - (PD)&lt;br&gt;
-				Tel: 049.66.78.42</t>
+Via P. D'Abano 14&lt;br&gt;
+35031 - Abano Terme - (PD)&lt;br&gt;
+Tel: 049.66.78.42</t>
   </si>
   <si>
     <t xml:space="preserve">SEDE SECONDARIA&lt;br&gt;
@@ -308,9 +391,12 @@
 				35036 - Montegrotto Terme - (PD)</t>
   </si>
   <si>
+    <t xml:space="preserve">вторичный офис &lt;br&gt; Piazzale  Stazione&lt;br&gt;     35036 - Montegrotto Terme – (PD)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SECONDARY OFFICE&lt;br&gt;
-				viale Stazione&lt;br&gt;
-				35036 - Montegrotto Terme - (PD)</t>
+viale Stazione&lt;br&gt;
+35036 - Montegrotto Terme - (PD)</t>
   </si>
 </sst>
 </file>
@@ -320,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -343,13 +429,41 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -361,7 +475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,25 +499,118 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Normal" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -414,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -433,10 +640,10 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -447,333 +654,417 @@
       <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="959.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="918.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="676.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>57</v>
+        <v>74</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="190.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="285" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="217.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>